<commit_message>
detail Info almost finish
</commit_message>
<xml_diff>
--- a/config/fm_기능정리.xlsx
+++ b/config/fm_기능정리.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\06.dfm\production\factoryModelerProduction\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F9DB75-28DA-4694-8DC7-9FE732E45231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B42D786-89F5-4AEC-8235-93483DB2675D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="2856" windowWidth="11208" windowHeight="11736" xr2:uid="{312DCB01-3ECF-4BDB-BD2E-FB7916E44140}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{312DCB01-3ECF-4BDB-BD2E-FB7916E44140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -591,7 +591,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>

</xml_diff>